<commit_message>
- add 3 form pages - page 2 e 3 only html/scss
</commit_message>
<xml_diff>
--- a/nutritional-data-visualization/src/data/vegan_dataset.xlsx
+++ b/nutritional-data-visualization/src/data/vegan_dataset.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="652" documentId="13_ncr:1_{8636283F-4200-48B0-8C04-7D8A10333072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C31330C-0A15-4697-89D1-4AD899C8233D}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUANTODECADACOISA" sheetId="6" r:id="rId1"/>
@@ -2360,6 +2360,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6650,9 +6654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>